<commit_message>
Fixed ADC readings quality
Re-configured ADC to use internal Vref, added filtering for ADC data, added hysteresis for ADC thresholds
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -15,6 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -64,7 +67,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -367,56 +370,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>0.17</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="B1">
         <v>255</v>
       </c>
       <c r="C1">
         <f>ROUND(B1*A1,0)</f>
-        <v>43</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>11</v>
+        <v>10.65</v>
       </c>
       <c r="B3" s="3">
         <f>A3*A4/(A4+A5)</f>
-        <v>3.6666666666666665</v>
+        <v>0.50714285714285712</v>
       </c>
       <c r="C3">
         <f>ROUND(B3*1024/A6,0)</f>
-        <v>736</v>
-      </c>
-      <c r="D3">
-        <f>ROUND(C3/4,0)</f>
-        <v>184</v>
+        <v>472</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>5.0999999999999996</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More RR features, batt from VTR
Added playback review reverse with record button, added battery charge level pickup from serial transmission from VTR, updated voltage LUT for input supply measurement, updated camera power calculation to prevent false "camera off" flags on low battery, dropped ATmega48 support, updated README, some code refactoring
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -67,7 +67,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -370,9 +370,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -390,15 +392,15 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>10.65</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="B3" s="3">
         <f>A3*A4/(A4+A5)</f>
-        <v>0.50714285714285712</v>
+        <v>1.3333333333333334E-2</v>
       </c>
       <c r="C3">
         <f>ROUND(B3*1024/A6,0)</f>
-        <v>472</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -414,6 +416,15 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B8">
+        <f>A3/A8</f>
+        <v>0.56000000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>